<commit_message>
fix : khong the connect api
</commit_message>
<xml_diff>
--- a/document/UI.xlsx
+++ b/document/UI.xlsx
@@ -174,31 +174,7 @@
     <t>[0-&gt;100]</t>
   </si>
   <si>
-    <t>http://127.0.0.1:5000/api/model/knn?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
-  </si>
-  <si>
     <t>Ta có 4 model nên có 4 api và tham số của nó giống nhau</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/api/model/knn</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/api/model/rand</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/api/model/mlp</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/api/model/linear</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/api/model/rand?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/api/model/mlp?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:5000/api/model/linear?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
   </si>
   <si>
     <t>[2016-&gt;]</t>
@@ -296,6 +272,30 @@
   </si>
   <si>
     <t>Cái nào chưa có là t chưa training</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/knn?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/rand?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/mlp?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/linear?nam=2019&amp;thang=4&amp;vido=20.972612&amp;kinhdo=105.850008&amp;loai=Nhacap&amp;loaiwc=Khepkin&amp;dientich=20.0&amp;drmd=2.2&amp;kcdc=169.0&amp;chodexe=1&amp;gacxep=1</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/knn</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/rand</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/mlp</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/api/models/linear</t>
   </si>
 </sst>
 </file>
@@ -417,6 +417,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -428,13 +435,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1023,7 @@
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
@@ -1040,11 +1040,11 @@
       <c r="G5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="H5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
@@ -1058,13 +1058,13 @@
         <v>42</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+        <v>53</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
@@ -1078,13 +1078,13 @@
         <v>42</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+        <v>54</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
@@ -1098,13 +1098,13 @@
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
@@ -1118,15 +1118,15 @@
         <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
       <c r="K9" t="s">
-        <v>65</v>
-      </c>
-      <c r="O9" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
@@ -1140,15 +1140,15 @@
         <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
       <c r="K10" t="s">
-        <v>65</v>
-      </c>
-      <c r="O10" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
@@ -1164,11 +1164,11 @@
       <c r="G11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
@@ -1184,11 +1184,11 @@
       <c r="G12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
@@ -1204,11 +1204,11 @@
       <c r="G13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="H13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
@@ -1224,11 +1224,11 @@
       <c r="G14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
@@ -1244,11 +1244,11 @@
       <c r="G15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="H15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
@@ -1264,11 +1264,11 @@
       <c r="G16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="H16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
@@ -1284,11 +1284,11 @@
       <c r="G17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="H17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
@@ -1304,11 +1304,11 @@
       <c r="G18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="H18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
@@ -1324,11 +1324,11 @@
       <c r="G19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="H19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
@@ -1344,11 +1344,11 @@
       <c r="G20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="H20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
@@ -1364,11 +1364,11 @@
       <c r="G21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="H21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
@@ -1384,11 +1384,11 @@
       <c r="G22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="H22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
@@ -1404,11 +1404,11 @@
       <c r="G23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="H23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
@@ -1424,11 +1424,11 @@
       <c r="G24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="H24" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
@@ -1444,116 +1444,104 @@
       <c r="G25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H25" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="H25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I28" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="I31" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I51" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I62" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J62" s="10"/>
+      <c r="I62" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J62" s="5"/>
     </row>
     <row r="63" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
     </row>
     <row r="64" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I62:J64"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="H6:J6"/>
@@ -1564,6 +1552,18 @@
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="I62:J64"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I29" r:id="rId1"/>

</xml_diff>